<commit_message>
Final details on regional charts
</commit_message>
<xml_diff>
--- a/Dataset working directory_reg/POLICY regional.xlsx
+++ b/Dataset working directory_reg/POLICY regional.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="VALUES" sheetId="1" state="visible" r:id="rId2"/>
@@ -553,13 +553,13 @@
     <t xml:space="preserve">Polynesia</t>
   </si>
   <si>
+    <t xml:space="preserve">2/3</t>
+  </si>
+  <si>
     <t xml:space="preserve">0/3</t>
   </si>
   <si>
     <t xml:space="preserve">1/3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2/3</t>
   </si>
   <si>
     <t xml:space="preserve">3/3</t>
@@ -673,8 +673,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.0255102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.6173469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1788,38 +1788,38 @@
       <c r="A29" s="0" t="s">
         <v>176</v>
       </c>
-      <c r="B29" s="0" t="s">
-        <v>99</v>
+      <c r="B29" s="1" t="s">
+        <v>177</v>
       </c>
       <c r="C29" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="G29" s="0" t="s">
         <v>177</v>
       </c>
-      <c r="D29" s="0" t="s">
+      <c r="H29" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="I29" s="0" t="s">
         <v>177</v>
       </c>
-      <c r="E29" s="0" t="s">
+      <c r="J29" s="0" t="s">
         <v>177</v>
       </c>
-      <c r="F29" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="G29" s="0" t="s">
+      <c r="K29" s="0" t="s">
         <v>179</v>
       </c>
-      <c r="H29" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="I29" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="J29" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="K29" s="0" t="s">
-        <v>178</v>
-      </c>
       <c r="L29" s="0" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M29" s="0" t="s">
         <v>180</v>

</xml_diff>